<commit_message>
made formatting in spreadsheets more consistent. variable naming more consistent. Created raw data for SM10-2025, results. Procedure documented in SRD-sprint1.docx
</commit_message>
<xml_diff>
--- a/data/raw/SM10k-2023-raw.xlsx
+++ b/data/raw/SM10k-2023-raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_m\Documents\0. Code\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_m\Documents\0-Code\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CAEE851-2163-4371-9431-85689A5BFDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC950963-0752-44D8-B126-253C8DAA64FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{BA4345E5-0568-4AEB-A210-7A444EB3DB47}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="319">
   <si>
-    <t>rank-sm</t>
-  </si>
-  <si>
     <t>lastname</t>
   </si>
   <si>
@@ -860,9 +857,6 @@
     <t>Wasen-im-Emmental</t>
   </si>
   <si>
-    <t>s_per_km</t>
-  </si>
-  <si>
     <t>Stade-Geneve</t>
   </si>
   <si>
@@ -993,6 +987,12 @@
   </si>
   <si>
     <t>USY-_-Trilogie-Sport</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>s_per_k</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,28 +1384,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
         <v>162</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>163</v>
       </c>
-      <c r="F1" t="s">
-        <v>164</v>
-      </c>
       <c r="G1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H1" t="s">
-        <v>274</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1413,19 +1413,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
       <c r="D2">
         <v>1993</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G2">
         <v>1755</v>
@@ -1439,19 +1439,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>1992</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G3">
         <v>1762</v>
@@ -1465,19 +1465,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
       <c r="D4">
         <v>1989</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G4">
         <v>1767</v>
@@ -1491,19 +1491,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
       <c r="D5">
         <v>1995</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G5">
         <v>1781</v>
@@ -1517,19 +1517,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>1991</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G6">
         <v>1797</v>
@@ -1543,19 +1543,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
       </c>
       <c r="D7">
         <v>1996</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G7">
         <v>1805</v>
@@ -1569,19 +1569,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
       </c>
       <c r="D8">
         <v>1995</v>
       </c>
       <c r="E8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G8">
         <v>1816</v>
@@ -1595,19 +1595,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
       </c>
       <c r="D9">
         <v>2000</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G9">
         <v>1818</v>
@@ -1621,19 +1621,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10">
         <v>2002</v>
       </c>
       <c r="E10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G10">
         <v>1823</v>
@@ -1647,19 +1647,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
       </c>
       <c r="D11">
         <v>1992</v>
       </c>
       <c r="E11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G11">
         <v>1827</v>
@@ -1673,19 +1673,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
       </c>
       <c r="D12">
         <v>1999</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G12">
         <v>1832</v>
@@ -1699,19 +1699,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1996</v>
       </c>
       <c r="E13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G13">
         <v>1837</v>
@@ -1725,19 +1725,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
       </c>
       <c r="D14">
         <v>1994</v>
       </c>
       <c r="E14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G14">
         <v>1838</v>
@@ -1751,19 +1751,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
         <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
       </c>
       <c r="D15">
         <v>2003</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G15">
         <v>1862</v>
@@ -1777,19 +1777,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
       </c>
       <c r="D16">
         <v>1992</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G16">
         <v>1873</v>
@@ -1803,19 +1803,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
       </c>
       <c r="D17">
         <v>1996</v>
       </c>
       <c r="E17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G17">
         <v>1874</v>
@@ -1829,19 +1829,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
         <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
       </c>
       <c r="D18">
         <v>1994</v>
       </c>
       <c r="E18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G18">
         <v>1881</v>
@@ -1855,19 +1855,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
         <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
       </c>
       <c r="D19">
         <v>1999</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G19">
         <v>1895</v>
@@ -1881,19 +1881,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
       </c>
       <c r="D20">
         <v>1985</v>
       </c>
       <c r="E20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G20">
         <v>1898</v>
@@ -1907,19 +1907,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
         <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
       </c>
       <c r="D21">
         <v>2003</v>
       </c>
       <c r="E21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G21">
         <v>1900</v>
@@ -1933,19 +1933,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
       </c>
       <c r="D22">
         <v>1982</v>
       </c>
       <c r="E22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G22">
         <v>1903</v>
@@ -1959,19 +1959,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23">
         <v>1998</v>
       </c>
       <c r="E23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G23">
         <v>1905</v>
@@ -1985,19 +1985,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>42</v>
       </c>
       <c r="D24">
         <v>1992</v>
       </c>
       <c r="E24" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G24">
         <v>1906</v>
@@ -2011,19 +2011,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
         <v>43</v>
-      </c>
-      <c r="C25" t="s">
-        <v>44</v>
       </c>
       <c r="D25">
         <v>2001</v>
       </c>
       <c r="E25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G25">
         <v>1907</v>
@@ -2037,19 +2037,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26">
         <v>1996</v>
       </c>
       <c r="E26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G26">
         <v>1907</v>
@@ -2063,19 +2063,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
       </c>
       <c r="D27">
         <v>1999</v>
       </c>
       <c r="E27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G27">
         <v>1910</v>
@@ -2089,19 +2089,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
         <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
       </c>
       <c r="D28">
         <v>2000</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G28">
         <v>1911</v>
@@ -2115,19 +2115,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
       </c>
       <c r="D29">
         <v>2004</v>
       </c>
       <c r="E29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G29">
         <v>1914</v>
@@ -2141,19 +2141,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
         <v>52</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
       </c>
       <c r="D30">
         <v>2001</v>
       </c>
       <c r="E30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G30">
         <v>1915</v>
@@ -2167,19 +2167,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
         <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
       </c>
       <c r="D31">
         <v>1978</v>
       </c>
       <c r="E31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G31">
         <v>1917</v>
@@ -2193,19 +2193,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32">
         <v>1988</v>
       </c>
       <c r="E32" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G32">
         <v>1917</v>
@@ -2219,19 +2219,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33">
         <v>2003</v>
       </c>
       <c r="E33" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G33">
         <v>1918</v>
@@ -2245,19 +2245,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
         <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
       </c>
       <c r="D34">
         <v>1996</v>
       </c>
       <c r="E34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G34">
         <v>1918</v>
@@ -2271,19 +2271,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
         <v>60</v>
-      </c>
-      <c r="C35" t="s">
-        <v>61</v>
       </c>
       <c r="D35">
         <v>1999</v>
       </c>
       <c r="E35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G35">
         <v>1919</v>
@@ -2297,19 +2297,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
         <v>62</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
       </c>
       <c r="D36">
         <v>1987</v>
       </c>
       <c r="E36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F36" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G36">
         <v>1919</v>
@@ -2323,19 +2323,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
         <v>64</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
       </c>
       <c r="D37">
         <v>2004</v>
       </c>
       <c r="E37" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F37" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G37">
         <v>1926</v>
@@ -2349,19 +2349,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
         <v>66</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
       </c>
       <c r="D38">
         <v>1998</v>
       </c>
       <c r="E38" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G38">
         <v>1931</v>
@@ -2375,19 +2375,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39">
         <v>1995</v>
       </c>
       <c r="E39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G39">
         <v>1936</v>
@@ -2401,19 +2401,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40">
         <v>1986</v>
       </c>
       <c r="E40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G40">
         <v>1938</v>
@@ -2427,19 +2427,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" t="s">
         <v>70</v>
-      </c>
-      <c r="C41" t="s">
-        <v>71</v>
       </c>
       <c r="D41">
         <v>2000</v>
       </c>
       <c r="E41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G41">
         <v>1939</v>
@@ -2453,19 +2453,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
         <v>72</v>
-      </c>
-      <c r="C42" t="s">
-        <v>73</v>
       </c>
       <c r="D42">
         <v>2000</v>
       </c>
       <c r="E42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G42">
         <v>1943</v>
@@ -2479,19 +2479,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" t="s">
         <v>74</v>
-      </c>
-      <c r="C43" t="s">
-        <v>75</v>
       </c>
       <c r="D43">
         <v>1975</v>
       </c>
       <c r="E43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F43" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G43">
         <v>1944</v>
@@ -2505,19 +2505,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
         <v>76</v>
-      </c>
-      <c r="C44" t="s">
-        <v>77</v>
       </c>
       <c r="D44">
         <v>1993</v>
       </c>
       <c r="E44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G44">
         <v>1951</v>
@@ -2531,19 +2531,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" t="s">
         <v>78</v>
-      </c>
-      <c r="C45" t="s">
-        <v>79</v>
       </c>
       <c r="D45">
         <v>1992</v>
       </c>
       <c r="E45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G45">
         <v>1953</v>
@@ -2557,19 +2557,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
         <v>80</v>
-      </c>
-      <c r="C46" t="s">
-        <v>81</v>
       </c>
       <c r="D46">
         <v>1987</v>
       </c>
       <c r="E46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G46">
         <v>1954</v>
@@ -2583,19 +2583,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D47">
         <v>1999</v>
       </c>
       <c r="E47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G47">
         <v>1955</v>
@@ -2609,19 +2609,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" t="s">
         <v>83</v>
-      </c>
-      <c r="C48" t="s">
-        <v>84</v>
       </c>
       <c r="D48">
         <v>1987</v>
       </c>
       <c r="E48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F48" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G48">
         <v>1956</v>
@@ -2635,19 +2635,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C49" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D49">
         <v>2001</v>
       </c>
       <c r="E49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F49" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G49">
         <v>1959</v>
@@ -2661,19 +2661,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D50">
         <v>1984</v>
       </c>
       <c r="E50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G50">
         <v>1969</v>
@@ -2687,19 +2687,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
         <v>86</v>
-      </c>
-      <c r="C51" t="s">
-        <v>87</v>
       </c>
       <c r="D51">
         <v>1995</v>
       </c>
       <c r="E51" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G51">
         <v>1972</v>
@@ -2713,19 +2713,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
         <v>88</v>
-      </c>
-      <c r="C52" t="s">
-        <v>89</v>
       </c>
       <c r="D52">
         <v>2003</v>
       </c>
       <c r="E52" t="s">
+        <v>199</v>
+      </c>
+      <c r="F52" t="s">
         <v>200</v>
-      </c>
-      <c r="F52" t="s">
-        <v>201</v>
       </c>
       <c r="G52">
         <v>1976</v>
@@ -2739,19 +2739,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53">
         <v>2002</v>
       </c>
       <c r="E53" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G53">
         <v>1979</v>
@@ -2765,19 +2765,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
         <v>91</v>
-      </c>
-      <c r="C54" t="s">
-        <v>92</v>
       </c>
       <c r="D54">
         <v>1998</v>
       </c>
       <c r="E54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F54" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G54">
         <v>1982</v>
@@ -2791,19 +2791,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D55">
         <v>2004</v>
       </c>
       <c r="E55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G55">
         <v>1982</v>
@@ -2817,19 +2817,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" t="s">
         <v>94</v>
-      </c>
-      <c r="C56" t="s">
-        <v>95</v>
       </c>
       <c r="D56">
         <v>1998</v>
       </c>
       <c r="E56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G56">
         <v>1983</v>
@@ -2843,19 +2843,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" t="s">
         <v>96</v>
-      </c>
-      <c r="C57" t="s">
-        <v>97</v>
       </c>
       <c r="D57">
         <v>1987</v>
       </c>
       <c r="E57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F57" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G57">
         <v>1985</v>
@@ -2869,19 +2869,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58">
         <v>1979</v>
       </c>
       <c r="E58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F58" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G58">
         <v>1989</v>
@@ -2895,19 +2895,19 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
         <v>99</v>
-      </c>
-      <c r="C59" t="s">
-        <v>100</v>
       </c>
       <c r="D59">
         <v>1992</v>
       </c>
       <c r="E59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F59" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G59">
         <v>1993</v>
@@ -2921,19 +2921,19 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" t="s">
         <v>101</v>
-      </c>
-      <c r="C60" t="s">
-        <v>102</v>
       </c>
       <c r="D60">
         <v>2001</v>
       </c>
       <c r="E60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G60">
         <v>1993</v>
@@ -2947,19 +2947,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" t="s">
         <v>103</v>
-      </c>
-      <c r="C61" t="s">
-        <v>104</v>
       </c>
       <c r="D61">
         <v>1995</v>
       </c>
       <c r="E61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F61" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G61">
         <v>1997</v>
@@ -2973,19 +2973,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" t="s">
         <v>105</v>
-      </c>
-      <c r="C62" t="s">
-        <v>106</v>
       </c>
       <c r="D62">
         <v>1995</v>
       </c>
       <c r="E62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F62" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G62">
         <v>2001</v>
@@ -2999,19 +2999,19 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D63">
         <v>2003</v>
       </c>
       <c r="E63" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F63" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G63">
         <v>2001</v>
@@ -3025,19 +3025,19 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D64">
         <v>1996</v>
       </c>
       <c r="E64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F64" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G64">
         <v>2001</v>
@@ -3051,19 +3051,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D65">
         <v>2000</v>
       </c>
       <c r="E65" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G65">
         <v>2003</v>
@@ -3077,19 +3077,19 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" t="s">
         <v>109</v>
-      </c>
-      <c r="C66" t="s">
-        <v>110</v>
       </c>
       <c r="D66">
         <v>2004</v>
       </c>
       <c r="E66" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G66">
         <v>2008</v>
@@ -3103,19 +3103,19 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D67">
         <v>1976</v>
       </c>
       <c r="E67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F67" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G67">
         <v>2009</v>
@@ -3129,19 +3129,19 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D68">
         <v>1999</v>
       </c>
       <c r="E68" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F68" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G68">
         <v>2010</v>
@@ -3155,19 +3155,19 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D69">
         <v>1987</v>
       </c>
       <c r="E69" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F69" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G69">
         <v>2010</v>
@@ -3181,19 +3181,19 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" t="s">
         <v>114</v>
-      </c>
-      <c r="C70" t="s">
-        <v>115</v>
       </c>
       <c r="D70">
         <v>1990</v>
       </c>
       <c r="E70" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F70" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G70">
         <v>2011</v>
@@ -3207,19 +3207,19 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D71">
         <v>2004</v>
       </c>
       <c r="E71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G71">
         <v>2011</v>
@@ -3233,19 +3233,19 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C72" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D72">
         <v>1994</v>
       </c>
       <c r="E72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G72">
         <v>2013</v>
@@ -3259,19 +3259,19 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" t="s">
         <v>118</v>
-      </c>
-      <c r="C73" t="s">
-        <v>119</v>
       </c>
       <c r="D73">
         <v>2002</v>
       </c>
       <c r="E73" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F73" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G73">
         <v>2018</v>
@@ -3285,19 +3285,19 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D74">
         <v>1977</v>
       </c>
       <c r="E74" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G74">
         <v>2020</v>
@@ -3311,19 +3311,19 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D75">
         <v>2008</v>
       </c>
       <c r="E75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F75" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G75">
         <v>2021</v>
@@ -3337,19 +3337,19 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D76">
         <v>1977</v>
       </c>
       <c r="E76" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F76" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G76">
         <v>2023</v>
@@ -3363,19 +3363,19 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" t="s">
         <v>123</v>
-      </c>
-      <c r="C77" t="s">
-        <v>124</v>
       </c>
       <c r="D77">
         <v>2002</v>
       </c>
       <c r="E77" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F77" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G77">
         <v>2026</v>
@@ -3389,19 +3389,19 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" t="s">
         <v>125</v>
-      </c>
-      <c r="C78" t="s">
-        <v>126</v>
       </c>
       <c r="D78">
         <v>1973</v>
       </c>
       <c r="E78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F78" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G78">
         <v>2027</v>
@@ -3415,19 +3415,19 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" t="s">
         <v>127</v>
-      </c>
-      <c r="C79" t="s">
-        <v>128</v>
       </c>
       <c r="D79">
         <v>1991</v>
       </c>
       <c r="E79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F79" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G79">
         <v>2033</v>
@@ -3441,19 +3441,19 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" t="s">
         <v>129</v>
-      </c>
-      <c r="C80" t="s">
-        <v>130</v>
       </c>
       <c r="D80">
         <v>1999</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F80" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G80">
         <v>2033</v>
@@ -3467,19 +3467,19 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" t="s">
         <v>131</v>
-      </c>
-      <c r="C81" t="s">
-        <v>132</v>
       </c>
       <c r="D81">
         <v>2006</v>
       </c>
       <c r="E81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F81" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G81">
         <v>2037</v>
@@ -3493,19 +3493,19 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" t="s">
         <v>133</v>
-      </c>
-      <c r="C82" t="s">
-        <v>134</v>
       </c>
       <c r="D82">
         <v>1994</v>
       </c>
       <c r="E82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F82" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G82">
         <v>2040</v>
@@ -3519,19 +3519,19 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D83">
         <v>1998</v>
       </c>
       <c r="E83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F83" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G83">
         <v>2041</v>
@@ -3545,19 +3545,19 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D84">
         <v>2005</v>
       </c>
       <c r="E84" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F84" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G84">
         <v>2041</v>
@@ -3571,19 +3571,19 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>135</v>
+      </c>
+      <c r="C85" t="s">
         <v>136</v>
-      </c>
-      <c r="C85" t="s">
-        <v>137</v>
       </c>
       <c r="D85">
         <v>1981</v>
       </c>
       <c r="E85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F85" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G85">
         <v>2043</v>
@@ -3597,19 +3597,19 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" t="s">
         <v>138</v>
-      </c>
-      <c r="C86" t="s">
-        <v>139</v>
       </c>
       <c r="D86">
         <v>1998</v>
       </c>
       <c r="E86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G86">
         <v>2047</v>
@@ -3623,19 +3623,19 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C87" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D87">
         <v>1989</v>
       </c>
       <c r="E87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F87" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G87">
         <v>2053</v>
@@ -3649,19 +3649,19 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C88" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D88">
         <v>1999</v>
       </c>
       <c r="E88" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F88" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G88">
         <v>2056</v>
@@ -3675,19 +3675,19 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>141</v>
+      </c>
+      <c r="C89" t="s">
         <v>142</v>
-      </c>
-      <c r="C89" t="s">
-        <v>143</v>
       </c>
       <c r="D89">
         <v>1971</v>
       </c>
       <c r="E89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F89" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G89">
         <v>2057</v>
@@ -3701,19 +3701,19 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C90" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D90">
         <v>2003</v>
       </c>
       <c r="E90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F90" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G90">
         <v>2071</v>
@@ -3727,19 +3727,19 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>144</v>
+      </c>
+      <c r="C91" t="s">
         <v>145</v>
-      </c>
-      <c r="C91" t="s">
-        <v>146</v>
       </c>
       <c r="D91">
         <v>1975</v>
       </c>
       <c r="E91" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F91" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G91">
         <v>2073</v>
@@ -3753,19 +3753,19 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C92" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D92">
         <v>2006</v>
       </c>
       <c r="E92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F92" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G92">
         <v>2074</v>
@@ -3779,19 +3779,19 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D93">
         <v>1979</v>
       </c>
       <c r="E93" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F93" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G93">
         <v>2074</v>
@@ -3805,19 +3805,19 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>148</v>
+      </c>
+      <c r="C94" t="s">
         <v>149</v>
-      </c>
-      <c r="C94" t="s">
-        <v>150</v>
       </c>
       <c r="D94">
         <v>2001</v>
       </c>
       <c r="E94" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F94" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G94">
         <v>2078</v>
@@ -3831,19 +3831,19 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C95" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D95">
         <v>1991</v>
       </c>
       <c r="E95" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F95" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G95">
         <v>2082</v>
@@ -3857,19 +3857,19 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>151</v>
+      </c>
+      <c r="C96" t="s">
         <v>152</v>
-      </c>
-      <c r="C96" t="s">
-        <v>153</v>
       </c>
       <c r="D96">
         <v>1979</v>
       </c>
       <c r="E96" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F96" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G96">
         <v>2086</v>
@@ -3883,19 +3883,19 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C97" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D97">
         <v>1997</v>
       </c>
       <c r="E97" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G97">
         <v>2087</v>
@@ -3909,19 +3909,19 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" t="s">
         <v>155</v>
-      </c>
-      <c r="C98" t="s">
-        <v>156</v>
       </c>
       <c r="D98">
         <v>1982</v>
       </c>
       <c r="E98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F98" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G98">
         <v>2088</v>
@@ -3935,19 +3935,19 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D99">
         <v>1995</v>
       </c>
       <c r="E99" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G99">
         <v>2094</v>
@@ -3961,19 +3961,19 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>157</v>
+      </c>
+      <c r="C100" t="s">
         <v>158</v>
-      </c>
-      <c r="C100" t="s">
-        <v>159</v>
       </c>
       <c r="D100">
         <v>2006</v>
       </c>
       <c r="E100" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F100" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G100">
         <v>2097</v>
@@ -3987,19 +3987,19 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>159</v>
+      </c>
+      <c r="C101" t="s">
         <v>160</v>
-      </c>
-      <c r="C101" t="s">
-        <v>161</v>
       </c>
       <c r="D101">
         <v>1990</v>
       </c>
       <c r="E101" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F101" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G101">
         <v>2097</v>

</xml_diff>